<commit_message>
Remove redundant literature + update README.md
</commit_message>
<xml_diff>
--- a/CSA_help.xlsx
+++ b/CSA_help.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\EAGLE\repos\EHM\"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t xml:space="preserve">N </t>
   </si>
@@ -392,6 +392,32 @@
   </si>
   <si>
     <t>Calculated</t>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OUT(MIN)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [μA]</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -506,29 +532,29 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -813,10 +839,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R16"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -843,28 +870,28 @@
       <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="K1" s="4" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="K1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="Q1" s="4" t="s">
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="Q1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4"/>
+      <c r="R1" s="13"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2">
         <v>25</v>
@@ -872,16 +899,16 @@
       <c r="C2" s="2">
         <v>2.7</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
       <c r="Q2" s="3" t="s">
         <v>9</v>
       </c>
@@ -891,80 +918,80 @@
       <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="12">
         <v>200</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
       <c r="K3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="9">
+      <c r="L3" s="12">
         <v>110</v>
       </c>
-      <c r="M3" s="9"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
       <c r="Q3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="R3" s="1"/>
     </row>
     <row r="4" spans="1:18" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="14">
         <f>((C2/(POWER(2,A2)-1))*F3)/(C2/1000)</f>
-        <v>195.50342130987289</v>
-      </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="K4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" s="10">
+        <v>48.840048840048837</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="K4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="14">
         <f>((C2/(POWER(2,A2)-1))*L3)/(C2/1000)</f>
-        <v>107.52688172043011</v>
-      </c>
-      <c r="M4" s="10"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
+        <v>26.862026862026863</v>
+      </c>
+      <c r="M4" s="14"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
     </row>
     <row r="5" spans="1:18" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="9">
-        <v>200</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="6" t="s">
+      <c r="F5" s="12">
+        <v>50</v>
+      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="9">
-        <v>110</v>
-      </c>
-      <c r="M5" s="9"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
+      <c r="L5" s="12">
+        <v>30</v>
+      </c>
+      <c r="M5" s="12"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
     </row>
     <row r="7" spans="1:18" ht="15.6" x14ac:dyDescent="0.35">
       <c r="E7" s="3" t="s">
@@ -1002,38 +1029,38 @@
       <c r="E8" s="3">
         <v>10</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <f>(C2/(POWER(2,A2)-1))/(E8*F5*POWER(10,-9))</f>
-        <v>1319.6480938416421</v>
-      </c>
-      <c r="G8" s="5">
+        <v>1318.6813186813185</v>
+      </c>
+      <c r="G8" s="4">
         <f>C2/(E8*F3*POWER(10,-6))</f>
         <v>1350</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="6">
         <f>F8/(B2*POWER(10,-3))</f>
-        <v>52785.92375366568</v>
-      </c>
-      <c r="I8" s="8">
+        <v>52747.252747252736</v>
+      </c>
+      <c r="I8" s="6">
         <f>G8/(B2*POWER(10,-3))</f>
         <v>54000</v>
       </c>
       <c r="K8" s="3">
         <v>10</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="4">
         <f>(C2/(POWER(2,A2)-1))/(K8*L5*POWER(10,-9))</f>
-        <v>2399.3601706211675</v>
-      </c>
-      <c r="M8" s="5">
+        <v>2197.8021978021975</v>
+      </c>
+      <c r="M8" s="4">
         <f>C2/(K8*L3*POWER(10,-6))</f>
         <v>2454.545454545455</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="6">
         <f>L8/(B2*POWER(10,-3))</f>
-        <v>95974.406824846694</v>
-      </c>
-      <c r="O8" s="8">
+        <v>87912.087912087896</v>
+      </c>
+      <c r="O8" s="6">
         <f>M8/(B2*POWER(10,-3))</f>
         <v>98181.818181818191</v>
       </c>
@@ -1042,38 +1069,38 @@
       <c r="E9" s="3">
         <v>20</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <f>(C2/(POWER(2,A2)-1))/(E9*F5*POWER(10,-9))</f>
-        <v>659.82404692082105</v>
-      </c>
-      <c r="G9" s="5">
+        <v>659.34065934065927</v>
+      </c>
+      <c r="G9" s="4">
         <f>C2/(E9*F3*POWER(10,-6))</f>
         <v>675</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="6">
         <f>F9/(B2*POWER(10,-3))</f>
-        <v>26392.96187683284</v>
-      </c>
-      <c r="I9" s="8">
+        <v>26373.626373626368</v>
+      </c>
+      <c r="I9" s="6">
         <f>G9/(B2*POWER(10,-3))</f>
         <v>27000</v>
       </c>
       <c r="K9" s="3">
         <v>20</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="4">
         <f>(C2/(POWER(2,A2)-1))/(K9*L5*POWER(10,-9))</f>
-        <v>1199.6800853105838</v>
-      </c>
-      <c r="M9" s="5">
+        <v>1098.9010989010987</v>
+      </c>
+      <c r="M9" s="4">
         <f>C2/(K9*L3*POWER(10,-6))</f>
         <v>1227.2727272727275</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="6">
         <f>L9/(B2*POWER(10,-3))</f>
-        <v>47987.203412423347</v>
-      </c>
-      <c r="O9" s="8">
+        <v>43956.043956043948</v>
+      </c>
+      <c r="O9" s="6">
         <f>M9/(B2*POWER(10,-3))</f>
         <v>49090.909090909096</v>
       </c>
@@ -1082,38 +1109,38 @@
       <c r="E10" s="3">
         <v>50</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <f>(C2/(POWER(2,A2)-1))/(E10*F5*POWER(10,-9))</f>
-        <v>263.9296187683284</v>
-      </c>
-      <c r="G10" s="5">
+        <v>263.73626373626371</v>
+      </c>
+      <c r="G10" s="4">
         <f>C2/(E10*F3*POWER(10,-6))</f>
         <v>270</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="6">
         <f>F10/(B2*POWER(10,-3))</f>
-        <v>10557.184750733135</v>
-      </c>
-      <c r="I10" s="8">
+        <v>10549.450549450548</v>
+      </c>
+      <c r="I10" s="6">
         <f>G10/(B2*POWER(10,-3))</f>
         <v>10800</v>
       </c>
       <c r="K10" s="3">
         <v>50</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="4">
         <f>(C2/(POWER(2,A2)-1))/(K10*L5*POWER(10,-9))</f>
-        <v>479.87203412423349</v>
-      </c>
-      <c r="M10" s="5">
+        <v>439.56043956043953</v>
+      </c>
+      <c r="M10" s="4">
         <f>C2/(K10*L3*POWER(10,-6))</f>
         <v>490.90909090909099</v>
       </c>
-      <c r="N10" s="8">
+      <c r="N10" s="6">
         <f>L10/(B2*POWER(10,-3))</f>
-        <v>19194.88136496934</v>
-      </c>
-      <c r="O10" s="8">
+        <v>17582.41758241758</v>
+      </c>
+      <c r="O10" s="6">
         <f>M10/(B2*POWER(10,-3))</f>
         <v>19636.36363636364</v>
       </c>
@@ -1122,38 +1149,38 @@
       <c r="E11" s="3">
         <v>100</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <f>(C2/(POWER(2,A2)-1))/(E11*F5*POWER(10,-9))</f>
-        <v>131.9648093841642</v>
-      </c>
-      <c r="G11" s="5">
+        <v>131.86813186813185</v>
+      </c>
+      <c r="G11" s="4">
         <f>C2/(E11*F3*POWER(10,-6))</f>
         <v>135</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="6">
         <f>F11/(B2*POWER(10,-3))</f>
-        <v>5278.5923753665675</v>
-      </c>
-      <c r="I11" s="8">
+        <v>5274.7252747252742</v>
+      </c>
+      <c r="I11" s="6">
         <f>G11/(B2*POWER(10,-3))</f>
         <v>5400</v>
       </c>
       <c r="K11" s="3">
         <v>100</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="4">
         <f>(C2/(POWER(2,A2)-1))/(K11*L5*POWER(10,-9))</f>
-        <v>239.93601706211675</v>
-      </c>
-      <c r="M11" s="5">
+        <v>219.78021978021977</v>
+      </c>
+      <c r="M11" s="4">
         <f>C2/(K11*L3*POWER(10,-6))</f>
         <v>245.4545454545455</v>
       </c>
-      <c r="N11" s="8">
+      <c r="N11" s="6">
         <f>L11/(B2*POWER(10,-3))</f>
-        <v>9597.4406824846701</v>
-      </c>
-      <c r="O11" s="8">
+        <v>8791.20879120879</v>
+      </c>
+      <c r="O11" s="6">
         <f>M11/(B2*POWER(10,-3))</f>
         <v>9818.1818181818198</v>
       </c>
@@ -1162,38 +1189,38 @@
       <c r="E12" s="3">
         <v>200</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <f>(C2/(POWER(2,A2)-1))/(E12*F5*POWER(10,-9))</f>
-        <v>65.982404692082099</v>
-      </c>
-      <c r="G12" s="5">
+        <v>65.934065934065927</v>
+      </c>
+      <c r="G12" s="4">
         <f>C2/(E12*F3*POWER(10,-6))</f>
         <v>67.5</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="6">
         <f>F12/(B2*POWER(10,-3))</f>
-        <v>2639.2961876832837</v>
-      </c>
-      <c r="I12" s="8">
+        <v>2637.3626373626371</v>
+      </c>
+      <c r="I12" s="6">
         <f>G12/(B2*POWER(10,-3))</f>
         <v>2700</v>
       </c>
       <c r="K12" s="3">
         <v>200</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="4">
         <f>(C2/(POWER(2,A2)-1))/(K12*L5*POWER(10,-9))</f>
-        <v>119.96800853105837</v>
-      </c>
-      <c r="M12" s="5">
+        <v>109.89010989010988</v>
+      </c>
+      <c r="M12" s="4">
         <f>C2/(K12*L3*POWER(10,-6))</f>
         <v>122.72727272727275</v>
       </c>
-      <c r="N12" s="8">
+      <c r="N12" s="6">
         <f>L12/(B2*POWER(10,-3))</f>
-        <v>4798.7203412423351</v>
-      </c>
-      <c r="O12" s="8">
+        <v>4395.604395604395</v>
+      </c>
+      <c r="O12" s="6">
         <f>M12/(B2*POWER(10,-3))</f>
         <v>4909.0909090909099</v>
       </c>
@@ -1214,19 +1241,19 @@
       <c r="E14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="12">
         <v>10700</v>
       </c>
-      <c r="G14" s="9"/>
+      <c r="G14" s="12"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="K14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L14" s="9">
-        <v>9760</v>
-      </c>
-      <c r="M14" s="9"/>
+      <c r="L14" s="12">
+        <v>9310</v>
+      </c>
+      <c r="M14" s="12"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
     </row>
@@ -1234,38 +1261,62 @@
       <c r="E15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="11">
         <f>B2*POWER(10,-3)*F14</f>
         <v>267.5</v>
       </c>
-      <c r="G15" s="7"/>
+      <c r="G15" s="11"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="K15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L15" s="7">
+      <c r="L15" s="11">
         <f>B2*POWER(10,-3)*L14</f>
-        <v>244</v>
-      </c>
-      <c r="M15" s="7"/>
+        <v>232.75</v>
+      </c>
+      <c r="M15" s="11"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+    <row r="16" spans="1:18" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="E16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="11">
+        <f>IF(AND(F14&gt;H8,F14&lt;I8),E8,IF(AND(F14&gt;H9,F14&lt;I9),E9,IF(AND(F14&gt;H10,F14&lt;I10),E10,IF(AND(F14&gt;H11,F14&lt;I11),E11,IF(AND(F14&gt;H12,F14&lt;I12),E12,NA())))))</f>
+        <v>50</v>
+      </c>
+      <c r="G16" s="11"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
+      <c r="K16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L16" s="11">
+        <f>IF(AND(L14&gt;N8,L14&lt;O8),K8,IF(AND(L14&gt;N9,L14&lt;O9),K9,IF(AND(L14&gt;N10,L14&lt;O10),K10,IF(AND(L14&gt;N11,L14&lt;O11),K11,IF(AND(L14&gt;N12,L14&lt;O12),K12,NA())))))</f>
+        <v>100</v>
+      </c>
+      <c r="M16" s="11"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
     </row>
+    <row r="17" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="15">
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="F16:G16"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="L14:M14"/>
     <mergeCell ref="L15:M15"/>

</xml_diff>